<commit_message>
AF of BC single should be 0 not 100
</commit_message>
<xml_diff>
--- a/R/data_manipulated/190422_Attenuation_factors_manual.xlsx
+++ b/R/data_manipulated/190422_Attenuation_factors_manual.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/katinkakrahn/Documents/MSc_Katinka/R/data_manipulated/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C593734-168E-F54B-9D82-5ABE46E15BD8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{31C67708-C619-6642-B06D-2E3D2E3EBEFF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="780" yWindow="1000" windowWidth="27640" windowHeight="15500" xr2:uid="{01009505-9940-474D-8900-1391AD7BB7BA}"/>
   </bookViews>
@@ -468,8 +468,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5D7ED31A-0950-7B4A-A1DE-65DB6749EAE2}">
   <dimension ref="A1:G79"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A56" workbookViewId="0">
-      <selection activeCell="G54" sqref="G54:G59"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G1" sqref="G1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -532,7 +532,7 @@
         <v>1</v>
       </c>
       <c r="G3" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
@@ -553,7 +553,7 @@
         <v>1</v>
       </c>
       <c r="G4" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
@@ -574,7 +574,7 @@
         <v>1</v>
       </c>
       <c r="G5" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.2">
@@ -595,7 +595,7 @@
         <v>1</v>
       </c>
       <c r="G6" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.2">
@@ -616,7 +616,7 @@
         <v>1</v>
       </c>
       <c r="G7" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.2">
@@ -654,7 +654,7 @@
         <v>1</v>
       </c>
       <c r="G9" s="2">
-        <v>0.41997890083802081</v>
+        <v>0.41997890083802097</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.2">
@@ -1059,7 +1059,7 @@
         <v>1</v>
       </c>
       <c r="G28" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.2">
@@ -1080,7 +1080,7 @@
         <v>1</v>
       </c>
       <c r="G29" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.2">
@@ -1101,7 +1101,7 @@
         <v>1</v>
       </c>
       <c r="G30" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.2">
@@ -1122,7 +1122,7 @@
         <v>1</v>
       </c>
       <c r="G31" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.2">
@@ -1143,7 +1143,7 @@
         <v>1</v>
       </c>
       <c r="G32" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.2">
@@ -1164,7 +1164,7 @@
         <v>1</v>
       </c>
       <c r="G33" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.2">
@@ -1593,7 +1593,7 @@
         <v>1</v>
       </c>
       <c r="G54" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.2">
@@ -1614,7 +1614,7 @@
         <v>1</v>
       </c>
       <c r="G55" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.2">
@@ -1635,7 +1635,7 @@
         <v>1</v>
       </c>
       <c r="G56" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="57" spans="1:7" x14ac:dyDescent="0.2">
@@ -1656,7 +1656,7 @@
         <v>1</v>
       </c>
       <c r="G57" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.2">
@@ -1677,7 +1677,7 @@
         <v>1</v>
       </c>
       <c r="G58" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.2">
@@ -1698,7 +1698,7 @@
         <v>1</v>
       </c>
       <c r="G59" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="60" spans="1:7" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Better spacings between facets and font size
</commit_message>
<xml_diff>
--- a/R/data_manipulated/190422_Attenuation_factors_manual.xlsx
+++ b/R/data_manipulated/190422_Attenuation_factors_manual.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/katinkakrahn/Documents/MSc_Katinka/R/data_manipulated/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7C00904-4955-EF49-B817-19E567942605}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53C951CB-E801-AB44-915C-5DF77D94C26E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="780" yWindow="1000" windowWidth="27640" windowHeight="15500" xr2:uid="{01009505-9940-474D-8900-1391AD7BB7BA}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="254" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="262" uniqueCount="29">
   <si>
     <t>Compound</t>
   </si>
@@ -110,6 +110,18 @@
   </si>
   <si>
     <t>S_sing</t>
+  </si>
+  <si>
+    <t>Kd_ref</t>
+  </si>
+  <si>
+    <t>n_ref</t>
+  </si>
+  <si>
+    <t>delta_Kd</t>
+  </si>
+  <si>
+    <t>log_delta_Kd</t>
   </si>
 </sst>
 </file>
@@ -467,15 +479,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5D7ED31A-0950-7B4A-A1DE-65DB6749EAE2}">
-  <dimension ref="A1:F79"/>
+  <dimension ref="A1:J79"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J20" sqref="J20"/>
+    <sheetView tabSelected="1" topLeftCell="A61" workbookViewId="0">
+      <selection activeCell="L77" sqref="L77"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -492,10 +504,22 @@
         <v>3</v>
       </c>
       <c r="F1" t="s">
+        <v>25</v>
+      </c>
+      <c r="G1" t="s">
+        <v>26</v>
+      </c>
+      <c r="H1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="I1" t="s">
+        <v>27</v>
+      </c>
+      <c r="J1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -509,9 +533,13 @@
       <c r="E2" t="s">
         <v>7</v>
       </c>
-      <c r="F2" s="2"/>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="F2" s="1"/>
+      <c r="G2" t="s">
+        <v>7</v>
+      </c>
+      <c r="H2" s="2"/>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>8</v>
       </c>
@@ -527,11 +555,23 @@
       <c r="E3">
         <v>1</v>
       </c>
-      <c r="F3" s="3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="F3" s="1">
+        <v>13669.146330714711</v>
+      </c>
+      <c r="G3">
+        <v>1</v>
+      </c>
+      <c r="H3" s="3">
+        <f>D3/F3</f>
+        <v>1</v>
+      </c>
+      <c r="I3" s="1">
+        <f>F3-D3</f>
+        <v>0</v>
+      </c>
+      <c r="J3" s="1"/>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>9</v>
       </c>
@@ -547,11 +587,23 @@
       <c r="E4">
         <v>1</v>
       </c>
-      <c r="F4" s="3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="F4" s="1">
+        <v>734185.38170284254</v>
+      </c>
+      <c r="G4">
+        <v>1</v>
+      </c>
+      <c r="H4" s="3">
+        <f t="shared" ref="H4:H67" si="0">D4/F4</f>
+        <v>1</v>
+      </c>
+      <c r="I4" s="1">
+        <f t="shared" ref="I4:I67" si="1">F4-D4</f>
+        <v>0</v>
+      </c>
+      <c r="J4" s="1"/>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>10</v>
       </c>
@@ -567,11 +619,23 @@
       <c r="E5">
         <v>1</v>
       </c>
-      <c r="F5" s="3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="F5" s="1">
+        <v>399192.53402764595</v>
+      </c>
+      <c r="G5">
+        <v>1</v>
+      </c>
+      <c r="H5" s="3">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="I5" s="1">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="J5" s="1"/>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>11</v>
       </c>
@@ -587,11 +651,23 @@
       <c r="E6">
         <v>1</v>
       </c>
-      <c r="F6" s="3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="F6" s="1">
+        <v>748489.21906965622</v>
+      </c>
+      <c r="G6">
+        <v>1</v>
+      </c>
+      <c r="H6" s="3">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="I6" s="1">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="J6" s="1"/>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>12</v>
       </c>
@@ -607,11 +683,23 @@
       <c r="E7">
         <v>1</v>
       </c>
-      <c r="F7" s="3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="F7" s="1">
+        <v>1135493.1239381621</v>
+      </c>
+      <c r="G7">
+        <v>1</v>
+      </c>
+      <c r="H7" s="3">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="I7" s="1">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="J7" s="1"/>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>5</v>
       </c>
@@ -625,9 +713,15 @@
       <c r="E8" t="s">
         <v>7</v>
       </c>
-      <c r="F8" s="3"/>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="F8" s="1"/>
+      <c r="G8" t="s">
+        <v>7</v>
+      </c>
+      <c r="H8" s="3"/>
+      <c r="I8" s="1"/>
+      <c r="J8" s="1"/>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>8</v>
       </c>
@@ -643,12 +737,26 @@
       <c r="E9">
         <v>1</v>
       </c>
-      <c r="F9" s="3">
-        <f>D9/D3</f>
+      <c r="F9" s="1">
+        <v>13669.146330714711</v>
+      </c>
+      <c r="G9">
+        <v>1</v>
+      </c>
+      <c r="H9" s="3">
+        <f t="shared" si="0"/>
         <v>1.8326345745780525E-2</v>
       </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="I9" s="1">
+        <f t="shared" si="1"/>
+        <v>13418.640829008367</v>
+      </c>
+      <c r="J9" s="1">
+        <f t="shared" ref="J4:J67" si="2">LOG10(I9)</f>
+        <v>4.1277085284741579</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>9</v>
       </c>
@@ -664,12 +772,26 @@
       <c r="E10">
         <v>1</v>
       </c>
-      <c r="F10" s="3">
-        <f t="shared" ref="F10:F13" si="0">D10/D4</f>
+      <c r="F10" s="1">
+        <v>734185.38170284254</v>
+      </c>
+      <c r="G10">
+        <v>1</v>
+      </c>
+      <c r="H10" s="3">
+        <f t="shared" si="0"/>
         <v>1.5195382681074205E-4</v>
       </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="I10" s="1">
+        <f t="shared" si="1"/>
+        <v>734073.8194245043</v>
+      </c>
+      <c r="J10" s="1">
+        <f t="shared" si="2"/>
+        <v>5.8657397353339169</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>10</v>
       </c>
@@ -685,12 +807,26 @@
       <c r="E11">
         <v>1</v>
       </c>
-      <c r="F11" s="3">
+      <c r="F11" s="1">
+        <v>399192.53402764595</v>
+      </c>
+      <c r="G11">
+        <v>1</v>
+      </c>
+      <c r="H11" s="3">
         <f t="shared" si="0"/>
         <v>7.4421349920564192E-3</v>
       </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="I11" s="1">
+        <f t="shared" si="1"/>
+        <v>396221.68930159113</v>
+      </c>
+      <c r="J11" s="1">
+        <f t="shared" si="2"/>
+        <v>5.5979382452716306</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>11</v>
       </c>
@@ -706,12 +842,26 @@
       <c r="E12">
         <v>1</v>
       </c>
-      <c r="F12" s="3">
+      <c r="F12" s="1">
+        <v>748489.21906965622</v>
+      </c>
+      <c r="G12">
+        <v>1</v>
+      </c>
+      <c r="H12" s="3">
         <f t="shared" si="0"/>
         <v>7.237173070587688E-3</v>
       </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="I12" s="1">
+        <f t="shared" si="1"/>
+        <v>743072.27304978005</v>
+      </c>
+      <c r="J12" s="1">
+        <f t="shared" si="2"/>
+        <v>5.8710310563719261</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>12</v>
       </c>
@@ -727,12 +877,26 @@
       <c r="E13">
         <v>1</v>
       </c>
-      <c r="F13" s="3">
+      <c r="F13" s="1">
+        <v>1135493.1239381621</v>
+      </c>
+      <c r="G13">
+        <v>1</v>
+      </c>
+      <c r="H13" s="3">
         <f t="shared" si="0"/>
         <v>1.2834902540818757E-2</v>
       </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="I13" s="1">
+        <f t="shared" si="1"/>
+        <v>1120919.180356646</v>
+      </c>
+      <c r="J13" s="1">
+        <f t="shared" si="2"/>
+        <v>6.0495743005606579</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>5</v>
       </c>
@@ -746,9 +910,15 @@
       <c r="E14" t="s">
         <v>7</v>
       </c>
-      <c r="F14" s="3"/>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="F14" s="1"/>
+      <c r="G14" t="s">
+        <v>7</v>
+      </c>
+      <c r="H14" s="3"/>
+      <c r="I14" s="1"/>
+      <c r="J14" s="1"/>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>8</v>
       </c>
@@ -762,9 +932,26 @@
       <c r="E15" t="s">
         <v>7</v>
       </c>
-      <c r="F15" s="3"/>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="F15" s="1">
+        <v>13669.146330714711</v>
+      </c>
+      <c r="G15">
+        <v>1</v>
+      </c>
+      <c r="H15" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I15" s="1">
+        <f t="shared" si="1"/>
+        <v>13669.146330714711</v>
+      </c>
+      <c r="J15" s="1">
+        <f t="shared" si="2"/>
+        <v>4.1357413927363202</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>9</v>
       </c>
@@ -780,12 +967,26 @@
       <c r="E16">
         <v>3</v>
       </c>
-      <c r="F16" s="3">
-        <f>D16/D4</f>
+      <c r="F16" s="1">
+        <v>734185.38170284254</v>
+      </c>
+      <c r="G16">
+        <v>1</v>
+      </c>
+      <c r="H16" s="3">
+        <f t="shared" si="0"/>
         <v>1.8808162586542454E-3</v>
       </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="I16" s="1">
+        <f t="shared" si="1"/>
+        <v>732804.51390006952</v>
+      </c>
+      <c r="J16" s="1">
+        <f t="shared" si="2"/>
+        <v>5.8649881358178924</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>10</v>
       </c>
@@ -801,12 +1002,26 @@
       <c r="E17">
         <v>3</v>
       </c>
-      <c r="F17" s="3">
-        <f t="shared" ref="F17:F19" si="1">D17/D5</f>
+      <c r="F17" s="1">
+        <v>399192.53402764595</v>
+      </c>
+      <c r="G17">
+        <v>1</v>
+      </c>
+      <c r="H17" s="3">
+        <f t="shared" si="0"/>
         <v>3.4092083329146816E-2</v>
       </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="I17" s="1">
+        <f t="shared" si="1"/>
+        <v>385583.22889320215</v>
+      </c>
+      <c r="J17" s="1">
+        <f t="shared" si="2"/>
+        <v>5.5861181358180936</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>11</v>
       </c>
@@ -822,12 +1037,26 @@
       <c r="E18">
         <v>3</v>
       </c>
-      <c r="F18" s="3">
-        <f t="shared" si="1"/>
+      <c r="F18" s="1">
+        <v>748489.21906965622</v>
+      </c>
+      <c r="G18">
+        <v>1</v>
+      </c>
+      <c r="H18" s="3">
+        <f t="shared" si="0"/>
         <v>3.3906241000123308E-2</v>
       </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="I18" s="1">
+        <f t="shared" si="1"/>
+        <v>723110.76322188636</v>
+      </c>
+      <c r="J18" s="1">
+        <f t="shared" si="2"/>
+        <v>5.8592048258860894</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>12</v>
       </c>
@@ -843,12 +1072,26 @@
       <c r="E19">
         <v>3</v>
       </c>
-      <c r="F19" s="3">
-        <f t="shared" si="1"/>
+      <c r="F19" s="1">
+        <v>1135493.1239381621</v>
+      </c>
+      <c r="G19">
+        <v>1</v>
+      </c>
+      <c r="H19" s="3">
+        <f t="shared" si="0"/>
         <v>0.10940778418153242</v>
       </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="I19" s="1">
+        <f t="shared" si="1"/>
+        <v>1011261.3372947216</v>
+      </c>
+      <c r="J19" s="1">
+        <f t="shared" si="2"/>
+        <v>6.004863403541898</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>10</v>
       </c>
@@ -864,12 +1107,26 @@
       <c r="E20">
         <v>1</v>
       </c>
-      <c r="F20" s="3">
-        <f>D20/D5</f>
+      <c r="F20" s="1">
+        <v>399192.53402764595</v>
+      </c>
+      <c r="G20">
+        <v>1</v>
+      </c>
+      <c r="H20" s="3">
+        <f t="shared" si="0"/>
         <v>0.10217450178399003</v>
       </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="I20" s="1">
+        <f t="shared" si="1"/>
+        <v>358405.23574748274</v>
+      </c>
+      <c r="J20" s="1">
+        <f t="shared" si="2"/>
+        <v>5.5543743454087027</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>5</v>
       </c>
@@ -883,9 +1140,15 @@
       <c r="E21" t="s">
         <v>7</v>
       </c>
-      <c r="F21" s="3"/>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="F21" s="1"/>
+      <c r="G21" t="s">
+        <v>7</v>
+      </c>
+      <c r="H21" s="3"/>
+      <c r="I21" s="1"/>
+      <c r="J21" s="1"/>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>8</v>
       </c>
@@ -901,12 +1164,15 @@
       <c r="E22">
         <v>3</v>
       </c>
-      <c r="F22" s="3">
-        <f>D22/D3</f>
-        <v>1.5895710408499322E-2</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="F22" s="1"/>
+      <c r="H22" s="3"/>
+      <c r="I22" s="1">
+        <f t="shared" si="1"/>
+        <v>-217.28079160444213</v>
+      </c>
+      <c r="J22" s="1"/>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>9</v>
       </c>
@@ -922,12 +1188,15 @@
       <c r="E23">
         <v>3</v>
       </c>
-      <c r="F23" s="3">
-        <f t="shared" ref="F23:F26" si="2">D23/D4</f>
-        <v>2.0152683559554569E-4</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="F23" s="1"/>
+      <c r="H23" s="3"/>
+      <c r="I23" s="1">
+        <f t="shared" si="1"/>
+        <v>-147.95805671508171</v>
+      </c>
+      <c r="J23" s="1"/>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>10</v>
       </c>
@@ -943,12 +1212,15 @@
       <c r="E24">
         <v>3</v>
       </c>
-      <c r="F24" s="3">
-        <f t="shared" si="2"/>
-        <v>1.3085964620102816E-3</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="F24" s="1"/>
+      <c r="H24" s="3"/>
+      <c r="I24" s="1">
+        <f t="shared" si="1"/>
+        <v>-522.38193768949645</v>
+      </c>
+      <c r="J24" s="1"/>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>11</v>
       </c>
@@ -964,12 +1236,15 @@
       <c r="E25">
         <v>3</v>
       </c>
-      <c r="F25" s="3">
-        <f t="shared" si="2"/>
-        <v>5.0182855252727649E-4</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="F25" s="1"/>
+      <c r="H25" s="3"/>
+      <c r="I25" s="1">
+        <f t="shared" si="1"/>
+        <v>-375.61326138799711</v>
+      </c>
+      <c r="J25" s="1"/>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>12</v>
       </c>
@@ -985,12 +1260,15 @@
       <c r="E26">
         <v>3</v>
       </c>
-      <c r="F26" s="3">
-        <f t="shared" si="2"/>
-        <v>3.1192630353815226E-4</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="F26" s="1"/>
+      <c r="H26" s="3"/>
+      <c r="I26" s="1">
+        <f t="shared" si="1"/>
+        <v>-354.19017284301992</v>
+      </c>
+      <c r="J26" s="1"/>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>10</v>
       </c>
@@ -1006,12 +1284,15 @@
       <c r="E27">
         <v>3</v>
       </c>
-      <c r="F27" s="3">
-        <f>D27/D5</f>
-        <v>1.6736946694917453E-3</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="F27" s="1"/>
+      <c r="H27" s="3"/>
+      <c r="I27" s="1">
+        <f t="shared" si="1"/>
+        <v>-668.12641630297321</v>
+      </c>
+      <c r="J27" s="1"/>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>5</v>
       </c>
@@ -1027,11 +1308,23 @@
       <c r="E28">
         <v>1</v>
       </c>
-      <c r="F28" s="3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="F28" s="1">
+        <v>295.20620916549387</v>
+      </c>
+      <c r="G28">
+        <v>1</v>
+      </c>
+      <c r="H28" s="3">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="I28" s="1">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="J28" s="1"/>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>8</v>
       </c>
@@ -1047,11 +1340,23 @@
       <c r="E29">
         <v>1</v>
       </c>
-      <c r="F29" s="3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="F29" s="1">
+        <v>2952.9605021652105</v>
+      </c>
+      <c r="G29">
+        <v>1</v>
+      </c>
+      <c r="H29" s="3">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="I29" s="1">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="J29" s="1"/>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>9</v>
       </c>
@@ -1067,11 +1372,23 @@
       <c r="E30">
         <v>1</v>
       </c>
-      <c r="F30" s="3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="F30" s="1">
+        <v>44400.430241519498</v>
+      </c>
+      <c r="G30">
+        <v>1</v>
+      </c>
+      <c r="H30" s="3">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="I30" s="1">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="J30" s="1"/>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>10</v>
       </c>
@@ -1087,11 +1404,23 @@
       <c r="E31">
         <v>1</v>
       </c>
-      <c r="F31" s="3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="F31" s="1">
+        <v>33471.070071230293</v>
+      </c>
+      <c r="G31">
+        <v>1</v>
+      </c>
+      <c r="H31" s="3">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="I31" s="1">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="J31" s="1"/>
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>11</v>
       </c>
@@ -1107,11 +1436,23 @@
       <c r="E32">
         <v>1</v>
       </c>
-      <c r="F32" s="3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="F32" s="1">
+        <v>151232.9953825885</v>
+      </c>
+      <c r="G32">
+        <v>1</v>
+      </c>
+      <c r="H32" s="3">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="I32" s="1">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="J32" s="1"/>
+    </row>
+    <row r="33" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>12</v>
       </c>
@@ -1127,11 +1468,23 @@
       <c r="E33">
         <v>1</v>
       </c>
-      <c r="F33" s="3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="F33" s="1">
+        <v>127033.1764625411</v>
+      </c>
+      <c r="G33">
+        <v>1</v>
+      </c>
+      <c r="H33" s="3">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="I33" s="1">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="J33" s="1"/>
+    </row>
+    <row r="34" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>5</v>
       </c>
@@ -1145,9 +1498,12 @@
       <c r="E34" t="s">
         <v>7</v>
       </c>
-      <c r="F34" s="3"/>
-    </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="F34" s="1"/>
+      <c r="H34" s="3"/>
+      <c r="I34" s="1"/>
+      <c r="J34" s="1"/>
+    </row>
+    <row r="35" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>8</v>
       </c>
@@ -1161,9 +1517,12 @@
       <c r="E35" t="s">
         <v>7</v>
       </c>
-      <c r="F35" s="3"/>
-    </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="F35" s="1"/>
+      <c r="H35" s="3"/>
+      <c r="I35" s="1"/>
+      <c r="J35" s="1"/>
+    </row>
+    <row r="36" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>9</v>
       </c>
@@ -1177,9 +1536,12 @@
       <c r="E36" t="s">
         <v>7</v>
       </c>
-      <c r="F36" s="3"/>
-    </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="F36" s="1"/>
+      <c r="H36" s="3"/>
+      <c r="I36" s="1"/>
+      <c r="J36" s="1"/>
+    </row>
+    <row r="37" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>10</v>
       </c>
@@ -1195,12 +1557,26 @@
       <c r="E37">
         <v>1</v>
       </c>
-      <c r="F37" s="3">
-        <f>D37/D31</f>
+      <c r="F37" s="1">
+        <v>33471.070071230293</v>
+      </c>
+      <c r="G37">
+        <v>1</v>
+      </c>
+      <c r="H37" s="3">
+        <f t="shared" si="0"/>
         <v>5.1814515024402728E-2</v>
       </c>
-    </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="I37" s="1">
+        <f t="shared" si="1"/>
+        <v>31736.782808141696</v>
+      </c>
+      <c r="J37" s="1">
+        <f t="shared" si="2"/>
+        <v>4.5015628997506765</v>
+      </c>
+    </row>
+    <row r="38" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>11</v>
       </c>
@@ -1216,12 +1592,26 @@
       <c r="E38">
         <v>1</v>
       </c>
-      <c r="F38" s="3">
-        <f>D38/D32</f>
+      <c r="F38" s="1">
+        <v>151232.9953825885</v>
+      </c>
+      <c r="G38">
+        <v>1</v>
+      </c>
+      <c r="H38" s="3">
+        <f t="shared" si="0"/>
         <v>1.4122940418273076E-2</v>
       </c>
-    </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="I38" s="1">
+        <f t="shared" si="1"/>
+        <v>149097.14079952324</v>
+      </c>
+      <c r="J38" s="1">
+        <f t="shared" si="2"/>
+        <v>5.1734693151706619</v>
+      </c>
+    </row>
+    <row r="39" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>12</v>
       </c>
@@ -1237,12 +1627,26 @@
       <c r="E39">
         <v>1</v>
       </c>
-      <c r="F39" s="3">
-        <f>D39/D33</f>
+      <c r="F39" s="1">
+        <v>127033.1764625411</v>
+      </c>
+      <c r="G39">
+        <v>1</v>
+      </c>
+      <c r="H39" s="3">
+        <f t="shared" si="0"/>
         <v>3.672353298801212E-2</v>
       </c>
-    </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="I39" s="1">
+        <f t="shared" si="1"/>
+        <v>122368.069416147</v>
+      </c>
+      <c r="J39" s="1">
+        <f t="shared" si="2"/>
+        <v>5.0876681082877324</v>
+      </c>
+    </row>
+    <row r="40" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>5</v>
       </c>
@@ -1256,9 +1660,12 @@
       <c r="E40" t="s">
         <v>7</v>
       </c>
-      <c r="F40" s="3"/>
-    </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="F40" s="1"/>
+      <c r="H40" s="3"/>
+      <c r="I40" s="1"/>
+      <c r="J40" s="1"/>
+    </row>
+    <row r="41" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>8</v>
       </c>
@@ -1272,9 +1679,12 @@
       <c r="E41" t="s">
         <v>7</v>
       </c>
-      <c r="F41" s="3"/>
-    </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="F41" s="1"/>
+      <c r="H41" s="3"/>
+      <c r="I41" s="1"/>
+      <c r="J41" s="1"/>
+    </row>
+    <row r="42" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>9</v>
       </c>
@@ -1288,9 +1698,12 @@
       <c r="E42" t="s">
         <v>7</v>
       </c>
-      <c r="F42" s="3"/>
-    </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="F42" s="1"/>
+      <c r="H42" s="3"/>
+      <c r="I42" s="1"/>
+      <c r="J42" s="1"/>
+    </row>
+    <row r="43" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>10</v>
       </c>
@@ -1306,12 +1719,26 @@
       <c r="E43">
         <v>3</v>
       </c>
-      <c r="F43" s="3">
-        <f>D43/D31</f>
+      <c r="F43" s="1">
+        <v>33471.070071230293</v>
+      </c>
+      <c r="G43">
+        <v>1</v>
+      </c>
+      <c r="H43" s="3">
+        <f t="shared" si="0"/>
         <v>4.3930884060183702E-2</v>
       </c>
-    </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="I43" s="1">
+        <f t="shared" si="1"/>
+        <v>32000.656372560792</v>
+      </c>
+      <c r="J43" s="1">
+        <f t="shared" si="2"/>
+        <v>4.5051588863217109</v>
+      </c>
+    </row>
+    <row r="44" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>11</v>
       </c>
@@ -1327,12 +1754,26 @@
       <c r="E44">
         <v>3</v>
       </c>
-      <c r="F44" s="3">
-        <f t="shared" ref="F44:F45" si="3">D44/D32</f>
+      <c r="F44" s="1">
+        <v>151232.9953825885</v>
+      </c>
+      <c r="G44">
+        <v>1</v>
+      </c>
+      <c r="H44" s="3">
+        <f t="shared" si="0"/>
         <v>7.1527235157670304E-3</v>
       </c>
-    </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="I44" s="1">
+        <f t="shared" si="1"/>
+        <v>150151.26758015557</v>
+      </c>
+      <c r="J44" s="1">
+        <f t="shared" si="2"/>
+        <v>5.1765290028736164</v>
+      </c>
+    </row>
+    <row r="45" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>12</v>
       </c>
@@ -1348,12 +1789,26 @@
       <c r="E45">
         <v>3</v>
       </c>
-      <c r="F45" s="3">
-        <f t="shared" si="3"/>
+      <c r="F45" s="1">
+        <v>127033.1764625411</v>
+      </c>
+      <c r="G45">
+        <v>1</v>
+      </c>
+      <c r="H45" s="3">
+        <f t="shared" si="0"/>
         <v>3.142265264019703E-2</v>
       </c>
-    </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="I45" s="1">
+        <f t="shared" si="1"/>
+        <v>123041.45708477782</v>
+      </c>
+      <c r="J45" s="1">
+        <f t="shared" si="2"/>
+        <v>5.0900514655013396</v>
+      </c>
+    </row>
+    <row r="46" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>10</v>
       </c>
@@ -1369,12 +1824,26 @@
       <c r="E46">
         <v>1</v>
       </c>
-      <c r="F46" s="3">
-        <f>D46/D31</f>
+      <c r="F46" s="1">
+        <v>33471.070071230293</v>
+      </c>
+      <c r="G46">
+        <v>1</v>
+      </c>
+      <c r="H46" s="3">
+        <f t="shared" si="0"/>
         <v>0.2855480007002808</v>
       </c>
-    </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="I46" s="1">
+        <f t="shared" si="1"/>
+        <v>23913.472931091477</v>
+      </c>
+      <c r="J46" s="1">
+        <f t="shared" si="2"/>
+        <v>4.3786426528736628</v>
+      </c>
+    </row>
+    <row r="47" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>5</v>
       </c>
@@ -1388,9 +1857,12 @@
       <c r="E47" t="s">
         <v>7</v>
       </c>
-      <c r="F47" s="3"/>
-    </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="F47" s="1"/>
+      <c r="H47" s="3"/>
+      <c r="I47" s="1"/>
+      <c r="J47" s="1"/>
+    </row>
+    <row r="48" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>8</v>
       </c>
@@ -1406,12 +1878,26 @@
       <c r="E48">
         <v>3</v>
       </c>
-      <c r="F48" s="3">
-        <f>D48/D29</f>
+      <c r="F48" s="1">
+        <v>2952.9605021652105</v>
+      </c>
+      <c r="G48">
+        <v>1</v>
+      </c>
+      <c r="H48" s="3">
+        <f t="shared" si="0"/>
         <v>7.3580663014329015E-2</v>
       </c>
-    </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="I48" s="1">
+        <f t="shared" si="1"/>
+        <v>2735.6797105607684</v>
+      </c>
+      <c r="J48" s="1">
+        <f t="shared" si="2"/>
+        <v>3.4370652494521128</v>
+      </c>
+    </row>
+    <row r="49" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>9</v>
       </c>
@@ -1427,12 +1913,26 @@
       <c r="E49">
         <v>3</v>
       </c>
-      <c r="F49" s="3">
-        <f t="shared" ref="F49:F52" si="4">D49/D30</f>
+      <c r="F49" s="1">
+        <v>44400.430241519498</v>
+      </c>
+      <c r="G49">
+        <v>1</v>
+      </c>
+      <c r="H49" s="3">
+        <f t="shared" si="0"/>
         <v>3.332356373806575E-3</v>
       </c>
-    </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="I49" s="1">
+        <f t="shared" si="1"/>
+        <v>44252.472184804414</v>
+      </c>
+      <c r="J49" s="1">
+        <f t="shared" si="2"/>
+        <v>4.6459375377734622</v>
+      </c>
+    </row>
+    <row r="50" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>10</v>
       </c>
@@ -1448,12 +1948,26 @@
       <c r="E50">
         <v>3</v>
       </c>
-      <c r="F50" s="3">
-        <f t="shared" si="4"/>
+      <c r="F50" s="1">
+        <v>33471.070071230293</v>
+      </c>
+      <c r="G50">
+        <v>1</v>
+      </c>
+      <c r="H50" s="3">
+        <f t="shared" si="0"/>
         <v>1.5606968542619268E-2</v>
       </c>
-    </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="I50" s="1">
+        <f t="shared" si="1"/>
+        <v>32948.688133540796</v>
+      </c>
+      <c r="J50" s="1">
+        <f t="shared" si="2"/>
+        <v>4.5178381276491111</v>
+      </c>
+    </row>
+    <row r="51" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>11</v>
       </c>
@@ -1469,12 +1983,26 @@
       <c r="E51">
         <v>3</v>
       </c>
-      <c r="F51" s="3">
-        <f t="shared" si="4"/>
+      <c r="F51" s="1">
+        <v>151232.9953825885</v>
+      </c>
+      <c r="G51">
+        <v>1</v>
+      </c>
+      <c r="H51" s="3">
+        <f t="shared" si="0"/>
         <v>2.4836726961452592E-3</v>
       </c>
-    </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="I51" s="1">
+        <f t="shared" si="1"/>
+        <v>150857.3821212005</v>
+      </c>
+      <c r="J51" s="1">
+        <f t="shared" si="2"/>
+        <v>5.1785665669873655</v>
+      </c>
+    </row>
+    <row r="52" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
         <v>12</v>
       </c>
@@ -1490,12 +2018,26 @@
       <c r="E52">
         <v>3</v>
       </c>
-      <c r="F52" s="3">
-        <f t="shared" si="4"/>
+      <c r="F52" s="1">
+        <v>127033.1764625411</v>
+      </c>
+      <c r="G52">
+        <v>1</v>
+      </c>
+      <c r="H52" s="3">
+        <f t="shared" si="0"/>
         <v>2.7881706394034924E-3</v>
       </c>
-    </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="I52" s="1">
+        <f t="shared" si="1"/>
+        <v>126678.98628969808</v>
+      </c>
+      <c r="J52" s="1">
+        <f t="shared" si="2"/>
+        <v>5.1027045794034436</v>
+      </c>
+    </row>
+    <row r="53" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>10</v>
       </c>
@@ -1511,12 +2053,26 @@
       <c r="E53">
         <v>3</v>
       </c>
-      <c r="F53" s="3">
-        <f>D53/D31</f>
+      <c r="F53" s="1">
+        <v>33471.070071230293</v>
+      </c>
+      <c r="G53">
+        <v>1</v>
+      </c>
+      <c r="H53" s="3">
+        <f t="shared" si="0"/>
         <v>1.9961310316076637E-2</v>
       </c>
-    </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="I53" s="1">
+        <f t="shared" si="1"/>
+        <v>32802.943654927323</v>
+      </c>
+      <c r="J53" s="1">
+        <f t="shared" si="2"/>
+        <v>4.515912817971711</v>
+      </c>
+    </row>
+    <row r="54" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
         <v>5</v>
       </c>
@@ -1532,11 +2088,23 @@
       <c r="E54">
         <v>1</v>
       </c>
-      <c r="F54" s="3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="F54" s="1">
+        <v>1870.2688625909966</v>
+      </c>
+      <c r="G54">
+        <v>1</v>
+      </c>
+      <c r="H54" s="3">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="I54" s="1">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="J54" s="1"/>
+    </row>
+    <row r="55" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
         <v>8</v>
       </c>
@@ -1552,11 +2120,23 @@
       <c r="E55">
         <v>1</v>
       </c>
-      <c r="F55" s="3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="F55" s="1">
+        <v>232.00975392056634</v>
+      </c>
+      <c r="G55">
+        <v>1</v>
+      </c>
+      <c r="H55" s="3">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="I55" s="1">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="J55" s="1"/>
+    </row>
+    <row r="56" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
         <v>9</v>
       </c>
@@ -1572,11 +2152,23 @@
       <c r="E56">
         <v>1</v>
       </c>
-      <c r="F56" s="3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="F56" s="1">
+        <v>40446.803841601926</v>
+      </c>
+      <c r="G56">
+        <v>1</v>
+      </c>
+      <c r="H56" s="3">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="I56" s="1">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="J56" s="1"/>
+    </row>
+    <row r="57" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
         <v>10</v>
       </c>
@@ -1592,11 +2184,23 @@
       <c r="E57">
         <v>1</v>
       </c>
-      <c r="F57" s="3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="F57" s="1">
+        <v>4415.24175832949</v>
+      </c>
+      <c r="G57">
+        <v>1</v>
+      </c>
+      <c r="H57" s="3">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="I57" s="1">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="J57" s="1"/>
+    </row>
+    <row r="58" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
         <v>11</v>
       </c>
@@ -1612,11 +2216,23 @@
       <c r="E58">
         <v>1</v>
       </c>
-      <c r="F58" s="3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="F58" s="1">
+        <v>23125.611074523447</v>
+      </c>
+      <c r="G58">
+        <v>1</v>
+      </c>
+      <c r="H58" s="3">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="I58" s="1">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="J58" s="1"/>
+    </row>
+    <row r="59" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
         <v>12</v>
       </c>
@@ -1632,11 +2248,23 @@
       <c r="E59">
         <v>1</v>
       </c>
-      <c r="F59" s="3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="F59" s="1">
+        <v>8357.2784876159021</v>
+      </c>
+      <c r="G59">
+        <v>1</v>
+      </c>
+      <c r="H59" s="3">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="I59" s="1">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="J59" s="1"/>
+    </row>
+    <row r="60" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
         <v>5</v>
       </c>
@@ -1650,9 +2278,12 @@
       <c r="E60" t="s">
         <v>7</v>
       </c>
-      <c r="F60" s="3"/>
-    </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="F60" s="1"/>
+      <c r="H60" s="3"/>
+      <c r="I60" s="1"/>
+      <c r="J60" s="1"/>
+    </row>
+    <row r="61" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
         <v>8</v>
       </c>
@@ -1668,12 +2299,26 @@
       <c r="E61">
         <v>1</v>
       </c>
-      <c r="F61" s="3">
-        <f>D61/D55</f>
+      <c r="F61" s="1">
+        <v>232.00975392056634</v>
+      </c>
+      <c r="G61">
+        <v>1</v>
+      </c>
+      <c r="H61" s="3">
+        <f t="shared" si="0"/>
         <v>0.66392641304136424</v>
       </c>
-    </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="I61" s="1">
+        <f t="shared" si="1"/>
+        <v>77.972350209475138</v>
+      </c>
+      <c r="J61" s="1">
+        <f t="shared" si="2"/>
+        <v>1.8919406247378447</v>
+      </c>
+    </row>
+    <row r="62" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
         <v>9</v>
       </c>
@@ -1689,12 +2334,26 @@
       <c r="E62">
         <v>1</v>
       </c>
-      <c r="F62" s="3">
-        <f t="shared" ref="F62:F65" si="5">D62/D56</f>
+      <c r="F62" s="1">
+        <v>40446.803841601926</v>
+      </c>
+      <c r="G62">
+        <v>1</v>
+      </c>
+      <c r="H62" s="3">
+        <f t="shared" si="0"/>
         <v>4.0087237763440356E-3</v>
       </c>
-    </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="I62" s="1">
+        <f t="shared" si="1"/>
+        <v>40284.663777364971</v>
+      </c>
+      <c r="J62" s="1">
+        <f t="shared" si="2"/>
+        <v>4.6051397432998034</v>
+      </c>
+    </row>
+    <row r="63" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
         <v>10</v>
       </c>
@@ -1710,12 +2369,26 @@
       <c r="E63">
         <v>1</v>
       </c>
-      <c r="F63" s="3">
-        <f t="shared" si="5"/>
+      <c r="F63" s="1">
+        <v>4415.24175832949</v>
+      </c>
+      <c r="G63">
+        <v>1</v>
+      </c>
+      <c r="H63" s="3">
+        <f t="shared" si="0"/>
         <v>0.12139993914820159</v>
       </c>
-    </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="I63" s="1">
+        <f t="shared" si="1"/>
+        <v>3879.2316775436911</v>
+      </c>
+      <c r="J63" s="1">
+        <f t="shared" si="2"/>
+        <v>3.5887457175413342</v>
+      </c>
+    </row>
+    <row r="64" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
         <v>11</v>
       </c>
@@ -1731,12 +2404,26 @@
       <c r="E64">
         <v>1</v>
       </c>
-      <c r="F64" s="3">
-        <f t="shared" si="5"/>
+      <c r="F64" s="1">
+        <v>23125.611074523447</v>
+      </c>
+      <c r="G64">
+        <v>1</v>
+      </c>
+      <c r="H64" s="3">
+        <f t="shared" si="0"/>
         <v>2.066583523804123E-2</v>
       </c>
-    </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="I64" s="1">
+        <f t="shared" si="1"/>
+        <v>22647.701006278323</v>
+      </c>
+      <c r="J64" s="1">
+        <f t="shared" si="2"/>
+        <v>4.3550241228626723</v>
+      </c>
+    </row>
+    <row r="65" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
         <v>12</v>
       </c>
@@ -1752,12 +2439,26 @@
       <c r="E65">
         <v>1</v>
       </c>
-      <c r="F65" s="3">
-        <f t="shared" si="5"/>
+      <c r="F65" s="1">
+        <v>8357.2784876159021</v>
+      </c>
+      <c r="G65">
+        <v>1</v>
+      </c>
+      <c r="H65" s="3">
+        <f t="shared" si="0"/>
         <v>9.7133808957873269E-2</v>
       </c>
-    </row>
-    <row r="66" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="I65" s="1">
+        <f t="shared" si="1"/>
+        <v>7545.5041955920751</v>
+      </c>
+      <c r="J65" s="1">
+        <f t="shared" si="2"/>
+        <v>3.8776882649263782</v>
+      </c>
+    </row>
+    <row r="66" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
         <v>5</v>
       </c>
@@ -1773,12 +2474,26 @@
       <c r="E66">
         <v>2</v>
       </c>
-      <c r="F66" s="3">
-        <f>D66/D54</f>
+      <c r="F66" s="1">
+        <v>1870.2688625909966</v>
+      </c>
+      <c r="G66">
+        <v>1</v>
+      </c>
+      <c r="H66" s="3">
+        <f t="shared" si="0"/>
         <v>8.2036679927950398E-2</v>
       </c>
-    </row>
-    <row r="67" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="I66" s="1">
+        <f t="shared" si="1"/>
+        <v>1716.8382145314072</v>
+      </c>
+      <c r="J66" s="1">
+        <f t="shared" si="2"/>
+        <v>3.2347293715460435</v>
+      </c>
+    </row>
+    <row r="67" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
         <v>8</v>
       </c>
@@ -1789,9 +2504,12 @@
       <c r="E67" t="s">
         <v>7</v>
       </c>
-      <c r="F67" s="3"/>
-    </row>
-    <row r="68" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="F67" s="1"/>
+      <c r="H67" s="3"/>
+      <c r="I67" s="1"/>
+      <c r="J67" s="1"/>
+    </row>
+    <row r="68" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
         <v>9</v>
       </c>
@@ -1802,9 +2520,12 @@
       <c r="E68" t="s">
         <v>7</v>
       </c>
-      <c r="F68" s="3"/>
-    </row>
-    <row r="69" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="F68" s="1"/>
+      <c r="H68" s="3"/>
+      <c r="I68" s="1"/>
+      <c r="J68" s="1"/>
+    </row>
+    <row r="69" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
         <v>10</v>
       </c>
@@ -1820,12 +2541,26 @@
       <c r="E69">
         <v>3</v>
       </c>
-      <c r="F69" s="3">
-        <f>D69/D57</f>
+      <c r="F69" s="1">
+        <v>4415.24175832949</v>
+      </c>
+      <c r="G69">
+        <v>1</v>
+      </c>
+      <c r="H69" s="3">
+        <f t="shared" ref="H69:H79" si="3">D69/F69</f>
         <v>0.15817866292526578</v>
       </c>
-    </row>
-    <row r="70" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="I69" s="1">
+        <f t="shared" ref="I68:I79" si="4">F69-D69</f>
+        <v>3716.8447205051316</v>
+      </c>
+      <c r="J69" s="1">
+        <f t="shared" ref="J68:J79" si="5">LOG10(I69)</f>
+        <v>3.5701744178521366</v>
+      </c>
+    </row>
+    <row r="70" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
         <v>11</v>
       </c>
@@ -1841,12 +2576,26 @@
       <c r="E70">
         <v>3</v>
       </c>
-      <c r="F70" s="3">
-        <f t="shared" ref="F70" si="6">D70/D58</f>
+      <c r="F70" s="1">
+        <v>23125.611074523447</v>
+      </c>
+      <c r="G70">
+        <v>1</v>
+      </c>
+      <c r="H70" s="3">
+        <f t="shared" si="3"/>
         <v>9.1935671005015634E-3</v>
       </c>
-    </row>
-    <row r="71" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="I70" s="1">
+        <f t="shared" si="4"/>
+        <v>22913.004217369715</v>
+      </c>
+      <c r="J70" s="1">
+        <f t="shared" si="5"/>
+        <v>4.3600820350422618</v>
+      </c>
+    </row>
+    <row r="71" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
         <v>12</v>
       </c>
@@ -1862,12 +2611,26 @@
       <c r="E71">
         <v>3</v>
       </c>
-      <c r="F71" s="3">
-        <f>D71/D59</f>
+      <c r="F71" s="1">
+        <v>8357.2784876159021</v>
+      </c>
+      <c r="G71">
+        <v>1</v>
+      </c>
+      <c r="H71" s="3">
+        <f t="shared" si="3"/>
         <v>0.10610299467469708</v>
       </c>
-    </row>
-    <row r="72" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="I71" s="1">
+        <f t="shared" si="4"/>
+        <v>7470.546212749432</v>
+      </c>
+      <c r="J71" s="1">
+        <f t="shared" si="5"/>
+        <v>3.8733523566361061</v>
+      </c>
+    </row>
+    <row r="72" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
         <v>10</v>
       </c>
@@ -1883,12 +2646,26 @@
       <c r="E72">
         <v>1</v>
       </c>
-      <c r="F72" s="3">
-        <f>D72/D57</f>
+      <c r="F72" s="1">
+        <v>4415.24175832949</v>
+      </c>
+      <c r="G72">
+        <v>1</v>
+      </c>
+      <c r="H72" s="3">
+        <f t="shared" si="3"/>
         <v>0.35060178073371484</v>
       </c>
-    </row>
-    <row r="73" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="I72" s="1">
+        <f t="shared" si="4"/>
+        <v>2867.2501354893129</v>
+      </c>
+      <c r="J72" s="1">
+        <f t="shared" si="5"/>
+        <v>3.4574655819329219</v>
+      </c>
+    </row>
+    <row r="73" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
         <v>5</v>
       </c>
@@ -1902,9 +2679,12 @@
       <c r="E73" t="s">
         <v>7</v>
       </c>
-      <c r="F73" s="3"/>
-    </row>
-    <row r="74" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="F73" s="1"/>
+      <c r="H73" s="3"/>
+      <c r="I73" s="1"/>
+      <c r="J73" s="1"/>
+    </row>
+    <row r="74" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
         <v>8</v>
       </c>
@@ -1920,12 +2700,26 @@
       <c r="E74">
         <v>3</v>
       </c>
-      <c r="F74" s="3">
-        <f>D74/D55</f>
+      <c r="F74" s="1">
+        <v>232.00975392056634</v>
+      </c>
+      <c r="G74">
+        <v>1</v>
+      </c>
+      <c r="H74" s="3">
+        <f t="shared" si="3"/>
         <v>0.93651576251760948</v>
       </c>
-    </row>
-    <row r="75" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="I74" s="1">
+        <f t="shared" si="4"/>
+        <v>14.72896231612421</v>
+      </c>
+      <c r="J74" s="1">
+        <f t="shared" si="5"/>
+        <v>1.1681721510343628</v>
+      </c>
+    </row>
+    <row r="75" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
         <v>9</v>
       </c>
@@ -1941,12 +2735,26 @@
       <c r="E75">
         <v>3</v>
       </c>
-      <c r="F75" s="3">
-        <f t="shared" ref="F75:F78" si="7">D75/D56</f>
+      <c r="F75" s="1">
+        <v>40446.803841601926</v>
+      </c>
+      <c r="G75">
+        <v>1</v>
+      </c>
+      <c r="H75" s="3">
+        <f t="shared" si="3"/>
         <v>3.6580901990307109E-3</v>
       </c>
-    </row>
-    <row r="76" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="I75" s="1">
+        <f t="shared" si="4"/>
+        <v>40298.845784886842</v>
+      </c>
+      <c r="J75" s="1">
+        <f t="shared" si="5"/>
+        <v>4.6052926075199423</v>
+      </c>
+    </row>
+    <row r="76" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
         <v>10</v>
       </c>
@@ -1962,12 +2770,26 @@
       <c r="E76">
         <v>3</v>
       </c>
-      <c r="F76" s="3">
-        <f t="shared" si="7"/>
+      <c r="F76" s="1">
+        <v>4415.24175832949</v>
+      </c>
+      <c r="G76">
+        <v>1</v>
+      </c>
+      <c r="H76" s="3">
+        <f t="shared" si="3"/>
         <v>0.1183133260379246</v>
       </c>
-    </row>
-    <row r="77" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="I76" s="1">
+        <f t="shared" si="4"/>
+        <v>3892.8598206399938</v>
+      </c>
+      <c r="J76" s="1">
+        <f t="shared" si="5"/>
+        <v>3.5902687653368051</v>
+      </c>
+    </row>
+    <row r="77" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
         <v>11</v>
       </c>
@@ -1983,12 +2805,26 @@
       <c r="E77">
         <v>3</v>
       </c>
-      <c r="F77" s="3">
-        <f t="shared" si="7"/>
+      <c r="F77" s="1">
+        <v>23125.611074523447</v>
+      </c>
+      <c r="G77">
+        <v>1</v>
+      </c>
+      <c r="H77" s="3">
+        <f t="shared" si="3"/>
         <v>1.6242306427171348E-2</v>
       </c>
-    </row>
-    <row r="78" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="I77" s="1">
+        <f t="shared" si="4"/>
+        <v>22749.997813135451</v>
+      </c>
+      <c r="J77" s="1">
+        <f t="shared" si="5"/>
+        <v>4.3569813592461752</v>
+      </c>
+    </row>
+    <row r="78" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
         <v>12</v>
       </c>
@@ -2004,12 +2840,26 @@
       <c r="E78">
         <v>3</v>
       </c>
-      <c r="F78" s="3">
-        <f t="shared" si="7"/>
+      <c r="F78" s="1">
+        <v>8357.2784876159021</v>
+      </c>
+      <c r="G78">
+        <v>1</v>
+      </c>
+      <c r="H78" s="3">
+        <f t="shared" si="3"/>
         <v>4.2381042269666006E-2</v>
       </c>
-    </row>
-    <row r="79" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="I78" s="1">
+        <f t="shared" si="4"/>
+        <v>8003.0883147728819</v>
+      </c>
+      <c r="J78" s="1">
+        <f t="shared" si="5"/>
+        <v>3.9032576093976332</v>
+      </c>
+    </row>
+    <row r="79" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
         <v>10</v>
       </c>
@@ -2025,9 +2875,23 @@
       <c r="E79">
         <v>3</v>
       </c>
-      <c r="F79" s="3">
-        <f>D79/D57</f>
+      <c r="F79" s="1">
+        <v>4415.24175832949</v>
+      </c>
+      <c r="G79">
+        <v>1</v>
+      </c>
+      <c r="H79" s="3">
+        <f t="shared" si="3"/>
         <v>0.15132272543004743</v>
+      </c>
+      <c r="I79" s="1">
+        <f t="shared" si="4"/>
+        <v>3747.1153420265168</v>
+      </c>
+      <c r="J79" s="1">
+        <f t="shared" si="5"/>
+        <v>3.5736970615578167</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Manuscript is ready now
</commit_message>
<xml_diff>
--- a/R/data_manipulated/190422_Attenuation_factors_manual.xlsx
+++ b/R/data_manipulated/190422_Attenuation_factors_manual.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10410"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10713"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/katinkakrahn/Documents/MSc_Katinka/R/data_manipulated/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/katinkakrahn/Documents/Skole/MSc_Katinka/R/data_manipulated/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7813E88A-8B6C-6C46-87FD-EA2A80484B3F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA059ADD-425A-5947-819D-4D6F783269CF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="780" yWindow="1000" windowWidth="27640" windowHeight="15500" xr2:uid="{01009505-9940-474D-8900-1391AD7BB7BA}"/>
   </bookViews>
@@ -128,9 +128,6 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="0.0000"/>
-  </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -164,7 +161,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -481,8 +478,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5D7ED31A-0950-7B4A-A1DE-65DB6749EAE2}">
   <dimension ref="A1:J79"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A59" workbookViewId="0">
-      <selection activeCell="H22" sqref="H22:H27"/>
+    <sheetView tabSelected="1" topLeftCell="A27" workbookViewId="0">
+      <selection activeCell="H44" sqref="H44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -594,7 +591,7 @@
         <v>1</v>
       </c>
       <c r="H4" s="3">
-        <f t="shared" ref="H4:H67" si="0">F4/D4</f>
+        <f t="shared" ref="H4:H66" si="0">F4/D4</f>
         <v>1</v>
       </c>
       <c r="I4" s="1">
@@ -971,7 +968,7 @@
         <v>1</v>
       </c>
       <c r="H16" s="3">
-        <f t="shared" si="0"/>
+        <f>F16/D16</f>
         <v>531.68404696560651</v>
       </c>
       <c r="I16" s="1">
@@ -1758,7 +1755,7 @@
         <v>1</v>
       </c>
       <c r="H44" s="3">
-        <f t="shared" si="0"/>
+        <f>F44/D44</f>
         <v>139.80688583805323</v>
       </c>
       <c r="I44" s="1">
@@ -2545,7 +2542,7 @@
         <v>1</v>
       </c>
       <c r="H69" s="3">
-        <f t="shared" ref="H68:H79" si="3">F69/D69</f>
+        <f t="shared" ref="H69:H79" si="3">F69/D69</f>
         <v>6.3219651848521892</v>
       </c>
       <c r="I69" s="1">

</xml_diff>